<commit_message>
Finshed updating trends paper for new bootstrapping
</commit_message>
<xml_diff>
--- a/trends/temp/table2.xlsx
+++ b/trends/temp/table2.xlsx
@@ -28,40 +28,40 @@
     <t>proportion drinking</t>
   </si>
   <si>
-    <t>(0.01)</t>
-  </si>
-  <si>
-    <t>(0.71)</t>
-  </si>
-  <si>
     <t>(0.2)</t>
   </si>
   <si>
-    <t>(0.48)</t>
-  </si>
-  <si>
     <t>(0.46)</t>
   </si>
   <si>
-    <t>(0.02)</t>
-  </si>
-  <si>
-    <t>(0.42)</t>
-  </si>
-  <si>
-    <t>(0.49)</t>
-  </si>
-  <si>
-    <t>(0.65)</t>
+    <t>(0.39)</t>
+  </si>
+  <si>
+    <t>(0.38)</t>
+  </si>
+  <si>
+    <t>(0.7)</t>
+  </si>
+  <si>
+    <t>(0.64)</t>
+  </si>
+  <si>
+    <t>(0.0)</t>
   </si>
   <si>
     <t>(0.03)</t>
   </si>
   <si>
-    <t>(0.4)</t>
-  </si>
-  <si>
-    <t>(0.0)</t>
+    <t>(0.16)</t>
+  </si>
+  <si>
+    <t>(0.12)</t>
+  </si>
+  <si>
+    <t>(0.06)</t>
+  </si>
+  <si>
+    <t>(0.47)</t>
   </si>
 </sst>
 </file>
@@ -467,10 +467,10 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -501,10 +501,10 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -535,10 +535,10 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -569,10 +569,10 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -603,10 +603,10 @@
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -637,10 +637,10 @@
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -671,10 +671,10 @@
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E15" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding proportion calcs to bootstrapping
</commit_message>
<xml_diff>
--- a/trends/temp/table2.xlsx
+++ b/trends/temp/table2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>year range</t>
   </si>
@@ -28,34 +28,52 @@
     <t>proportion drinking</t>
   </si>
   <si>
-    <t>(0.07)</t>
-  </si>
-  <si>
-    <t>(0.16)</t>
-  </si>
-  <si>
-    <t>(0.31)</t>
+    <t>(0.13)</t>
+  </si>
+  <si>
+    <t>(0.21)</t>
+  </si>
+  <si>
+    <t>(0.15)</t>
   </si>
   <si>
     <t>(0.01)</t>
   </si>
   <si>
-    <t>(0.15)</t>
-  </si>
-  <si>
-    <t>(0.28)</t>
-  </si>
-  <si>
-    <t>(0.11)</t>
-  </si>
-  <si>
-    <t>(0.0)</t>
-  </si>
-  <si>
-    <t>(0.12)</t>
+    <t>(0.81)</t>
+  </si>
+  <si>
+    <t>(0.26)</t>
+  </si>
+  <si>
+    <t>(0.3)</t>
   </si>
   <si>
     <t>(0.02)</t>
+  </si>
+  <si>
+    <t>(0.05)</t>
+  </si>
+  <si>
+    <t>(0.04)</t>
+  </si>
+  <si>
+    <t>(0.32)</t>
+  </si>
+  <si>
+    <t>(0.19)</t>
+  </si>
+  <si>
+    <t>(0.00004)</t>
+  </si>
+  <si>
+    <t>(0.00002)</t>
+  </si>
+  <si>
+    <t>(0.00000)</t>
+  </si>
+  <si>
+    <t>(0.00003)</t>
   </si>
 </sst>
 </file>
@@ -447,7 +465,7 @@
         <v>7.1</v>
       </c>
       <c r="E2">
-        <v>0.182</v>
+        <v>0.182455</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -464,7 +482,7 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -481,7 +499,7 @@
         <v>8</v>
       </c>
       <c r="E4">
-        <v>0.167</v>
+        <v>0.167269</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -495,10 +513,10 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -515,7 +533,7 @@
         <v>9.109999999999999</v>
       </c>
       <c r="E6">
-        <v>0.123</v>
+        <v>0.122975</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -529,10 +547,10 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -549,7 +567,7 @@
         <v>10.61</v>
       </c>
       <c r="E8">
-        <v>0.101</v>
+        <v>0.101189</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -563,10 +581,10 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -583,7 +601,7 @@
         <v>11.64</v>
       </c>
       <c r="E10">
-        <v>0.093</v>
+        <v>0.092802</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -597,10 +615,10 @@
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -617,7 +635,7 @@
         <v>11.22</v>
       </c>
       <c r="E12">
-        <v>0.097</v>
+        <v>0.09722799999999999</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -631,10 +649,10 @@
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -651,7 +669,7 @@
         <v>9.31</v>
       </c>
       <c r="E14">
-        <v>0.09</v>
+        <v>0.089807</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -665,10 +683,10 @@
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>